<commit_message>
HW5 Finished ( Inverter Delay )
</commit_message>
<xml_diff>
--- a/HW5/Results/Results_HW5_DigitalMos.xlsx
+++ b/HW5/Results/Results_HW5_DigitalMos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omer\Documents\GitHub\DigitalMosInteg.Circ.Design\HW5\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dersler\ITU\ELE\ELE-504E\HWs\DigitalMosInteg.Circ.Design\HW5\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF522226-1E09-43D1-B573-3A01B202CDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBBCCA2-273D-407A-B836-834736B91B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2070" yWindow="1725" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -178,14 +178,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,251 +468,252 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="3" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>